<commit_message>
Updated Codes, Data Sets & added Predictions
</commit_message>
<xml_diff>
--- a/Data Sets/Cleaned Text Hotel Reviews.xlsx
+++ b/Data Sets/Cleaned Text Hotel Reviews.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Dhaka Regency" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Ascott The Residence Dhaka" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4503,4 +4504,2753 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A390"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Cleaned Reviews</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>the ascott the residences dhaka very security n safety area at baridha diplomatic zonewe feel very comfortable therevery nice and well decorated meeting venueservice stuff are very professionally take care specially mr basher give us nice service</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>we are made meeting at nabiha restaurant at ascott the residence at dhaka very good looking  n nice decorated restaurant very good food n excellent service specially mr bashers very cordial n good service provide us</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>i had a fantastic experience at ascott the residence hotel in baridhara dhaka the hotels location inside the diplomatic zone is ideal the staff is incredibly professional and cordial with a special shoutout to mr bashar who provided exceptional service i highly recommend this place for a comfortable stay in dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">good food and service overall mr bashar was a good service provider to us during the business meeting our company has arranged our quarterly workshop here for the day and the overall experience has been good </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">our stay started with a warm welcome by an exceptional friendly staff at the hotel reception followed up with very nice and friendly people good food and relaxing atmosphere in the breakfast lounge many thanks to bashar sonia and kanniya for making our breakfast time memorable and pleasant and wearing the best cricket team shirts for the cricket world cup  best regards and good luck in wc from your friends in norway jan  una   </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>mr bashar was great at his service i enjoyed my stay here its  near to airport i was assisted and served with hospitality it was a wonderful experience here at this hotel besides its value for money</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ascott the residence dhaka really we feel my safety security home as like my own house room is very comfortable service stuff are very good specially mr bashar give me very easy to stay here  very tidy n clean hotel </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>comfortable stay with good staff eg mr bashar in the breakfast floor hotel in the diplomatic zone of dhaka those who are seeking to stay in the baridhara area for business or embassy workds can stay here</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the service was excellent we were served by their colleague mr bashar who was very hospitable and welcoming the environment was perfect for business meeting highly recommended for anyone to visit them for authentic experience </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>staff is very  nice and take care of every need of the guest mr bashar is once who has taken everything like im vegetarian so hotel provided me vegetarian food whenever i asked for it  i always recommend this hotel to my friend</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>the hotel is very beautiful the room is very tidy  the bed is very comfortable  the staff are all very accommodating  especially the room service is very good restaurant people are very good they gave very good service abul bashar is very good among them he is very flexible</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">good stay ascott residence hotel we are came our company joyton day long programme at serenity hall  very good event enjoy specially mr brasher give service  at nabiha restaurant at breakfasts  thanks </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">excellent service mr bashar help to prepared special tea ascott the residence dhaka i feel very comfortable n safety security as like my home room was very good staying food also good service stuff make very easy </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i have come over into dhaka and visited several places for eating as international traveller eating is very important for usthe hotel have one of the best eatery at dhaka the chef mr basher azmal and emon is really outdone himself by recreating all those delicious international cuisine in this hotel dining scene the meats are tenders the serving are done with meticulous attention and the seasoning was optimized for the experience of international tastenot just catering to local tounge creating perfect balance of taste which is very important hopefully for the next visit ill be able to meet them again and have another delightful experience </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>really happy with the accomodation of the hotel the hotel staff had a warm welcoming nature  the food and other facilities were excellent morning breakfast buffet was really good and mr bashar and the morning staff really helped a lot while we had our stay will definitely come back again all in all the hotel is located in the safest spot of the country will gladly recommend this place to anyone visiting dhaka from outside</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>the staff at the ascott was extremely hospitable and went out of their way to make you feel comfortable zannat basharr anowarr masud karniya disharri suvro tarik mehdi shafiq and allof the other staff members do a great job in creating a homely atmosphere</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>very good and kind service espacially mr bashar he has taken a very good care at the breakfast the hotel is located in a very friendly neighborhood good place people and service id would surely visit this hotel again in my next trip</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>homely environment nice service good food safe environment mr bashar was very cordial safe place for expat personnel as they have scanning facility in front of the gate nice housekeeping from the hotel crewm</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the best things about the ascott residence hotel dhaka an amazing teams whice ensure you  have your needsspecially mr brasher very professional and well known hospitality service mir  arfan and ms karnia gives very good service at breakfast thanks team to residence </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">very good service every staff were gender sensitive food quality was good room space was more than enough every time manager and other responsible person asked what need and they provide the support should have a swimming pool </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">food was great we had lunch with family ordered beef kadai mutton biroyani etc mr bashar served us with a smile nice ambiance and plesure experience  if youre near baridhara you can visit or stay here good place for friends  and family  </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">super management im highly happy with is and specially thanks to  abubakor munsi he is a nice man and caring  all the best ascott dhakathis hotel is very clean and staff all friendly i will come back again thanks </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ascottt the residenceh hotel i am very happy with there hospitality service    specially mr basher very good service provide us  mr mehedy also givehelping  good support  room n restaurant good n nice decoration we  are happy</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>thanks ascott resident hotel dhaka baridhara i have nice experience excellent service behaviour all staff accommodation is excellent thanks again ascott resident food was good one staf member mr bashir good service in breakfast time thanks</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>alcott the residents dhaka is a very safety  and security zone in baridhara diplomatic there was i fell very comfortable very clean nice organised hotelbuffet breakfast really good service stuff specially mr basher give special service  us</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>i am happy  to good service nice and comfortable enjoy with ascott residence dhaka very good food and service  specially mr brasher give me very easy to stayi will come again good safety n very clean hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">very good service and has a nice food in restaurants specially for mr bashan and karnia mehede give us good service in all time room is very clean and hotel area was very safety for me and my friend </t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>if you want to hold a small to medium range meeting they have a great meeting space if you want to have a business meeting with great food this place is what you are looking for ask for bashar to get even great service</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>the best thing about the place is its staff an amazing team which ensures you have a great experience and stay people like bashar in the restaurant go beyond the call of duty to take care of your needs</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i am a very frequent visitor to this hotel i am from kolkata and i used to come to dhaka very frequently and mostly i prefer to stay at ascott the residence the food comfort at the room is very satisfactory also the sincere hospitality of the staff like habib bhai made me feel more at ease </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>good food at nabihah restaurant and cafe and great service by mr basher  mr emon ascott hotel where its located is in a calm and peaceful part of the diplomatic enclave no noise pollution and a very safe area to stay in try the prawn malai curry and seasonal fruit cocktail it was delicious</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>comfortable hotel with very attentive service the location is in a diplomatic area away from commercial besides breakfast we ate our dinners at the hotel the food was very tasty with international and local dishes available</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">excellent hotel nice place to dine too particularly the sky top restaurantcordial staff and in particular i liked the hospitality and friendly guidance given by one of the hotel staff named mr anowar a room attendantwho took me on a  tour in and around the hoteland its facilities </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it was an amazing hospitality in a business event which was wonderfully organized by ascott the residence dhaka special service by mr basher mr mehedi and thier outstanding team thank you so very to all </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>very good hotel the staff are very nice and helpful they always ask how i am and are always game for a good conversation they always make sure that i am taken care of props especially to habib for the great service</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ascott the residence dhaka  mr basar was so cordial in response  he serviced in the japan embassy programme his behaviour and service are too good he is very active  and great in work  i wish him good luck </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>excellent food ambience got tremendous service from mehedi basar karnia khairul at japan embassy food  beverage was great outdoor catering is nice to have wish all the best to ascott palace</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>good roman good person i have a good time in the hotel very good servicethe hotel environment is good with spacious rooms and a delicious breakfastroom service is always prompt and attentive in bangladesh it makes me feel very happy</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i stayed  ascott residence hotel very comfortable room was very well decorates very safety n security full area   i enjoy as like my home  i am very happy with ascott food was very nice service stuff well very good service provide specially mr bher give nice support  mr emon special make coffee </t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hotel is very secured safe and good hospitality mr basar is prepared a very nice coffee he is also polite and gentle hotel is providing support as per the guest needs  resturant and its service is very good there is several items found here    all the best  </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>we are came to business by basudhara companywe stayed ascott residencehotel is very nice to stayvery good security n safety areawe stay very comfortablevery good service stuff are very friendlyspecially mr basher give us very easy to stayed</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i am very happy to ascott the residence dhakai stayed here very comfortablevery clean n oraganised hotel service stuff are frofesonalspecialy mr basher give me very good service at breakfasthe make coffee very nice </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>very good accommodation and service very homey the area is very safe and the food is very tasty especially mr bashar and abubakor thank you very much for always asking how i am and for the smiles every day</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>the ascott residence hotel was a wonderful experience in last visit best hotel in a dhaka cityroom was nice and very clean food options was very good  breakfast is very markable and deliciousthe staff are always smiles and welcoming the guests specially mr shafiq  from reception very helpful and  always look after methe hotel surround also very nice and attractive  im highly recommended ascott the hotel dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> i would definitely stay here again because i would like to extend my appreciation to all staff specially mr shafiq and mr abdullah on duty during our visit his responsibility pleasant helpful nature made our stay even more enjoyable his kind attentiveness to our needs and prompt assistance truly exemplified the epitome of exceptional service overall the combination of the outstanding service excellent facilities for reception room food and the warm hospitality of your staff made our stay at ascott residence hotel dhaka  i wholeheartedly recommend ascott hotel dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ascott the residence is a beautiful hotel  to visit in dhaka the breakfast is variety and delicious the staff of the hotel have a good costumer service i met mr bashar and mr emon that attended me very well in everything that i needed  full recommended </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i am very happy with ascott the residencei stayed there my company toshiba very nice hotel in dhakaroom is very nice well decorat very security n safety area in baridhaservice stuff very good specially mr basher give us very to stay here  thank you all </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the room is comfortable the staff is super friendly and helpful thank you very much to mr mehedi and mr bashar for their help  the hotel is clean organized and the staff keeps it all the time in perfect state </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the ascott the residence is in my opinion the best hotel in bangladesh i have stayed here before the hotel service and staff are excellent the restaurant and food is superb and in particular all staff from the cleaner to the manager are exceptional especially at the desk mr shafiq  habib abdullah were very helpful </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>our stay was really lovely  a comfortable room with air conditioning the staff were delightful and the food was delicious i would highly recommend this hotel particularly i have to mention that mr shafiq abdullah  islam were very helpful dhaka is a fantastic city with beautiful people  tranquil area</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>the hotel all good the room is comfortable ascott the residence dhaka is the best choice specially mrbashar give very good service bakery in dinner area is very well coffee is excelent staff have a good servicemind</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>i veryhappystaywithascotttheresidence dahai sayed herecouplesdayverynicecomfortableservicestuffareverynicespeceillymrbashergivemeverycomfortableaslo mr emonnms karniaservice good i comebackagain</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>peaceful location with caring staffs staffs are also flexible and accomodating to your requests a part of the city   gulshan  is just across the street if you are after shopping worth the deal and i would want to come back</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">good in hospitality and management well behaved team and fellows who cared guests requirements and tried to address their special need i appreciate their efforts specially support servic staff mr bashar who cared the event </t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ascott is conveniently located news our office services are outstanding mr bashar has been very friendly and served us exceptionally well professionalism and service really stands out safety and security is an added point as it is located in baridhara diplomatic zone</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>excellent service great hotel breakfast is impressive with brilliant service by mr bashar who makes you feel at home the rooms are exquisite and staff happy to help anytime with a smile great location tok</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">extremely comfortable stay with a bunch of motivated and happy staff  always going out of the way to meet our needs  very comfortable beds  clean  good food  special thanks to mr tareq salman    sonia and bashar for making us feel at home  i will highly recommend ascot if you are looking for a nice stay  </t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">food quality is good  with safety and security with hygienic lobby and room excellent behaviour staff specially mr bashar a good person  i feel free to contact any indian food service as i need i got really appreciate </t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>excellent service from hotel staff bashar nice place and atmosphere i am visiting for business the area is safe and comfortable i recommend the hotels in the area dinner was good but i recommend more variety on the menu</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">excellent hotel  i stay here long timei am very happy with ascott the residence hotel dhakamr bashar give me special service  he very well known this hospitalityfood is very  nice  very saefty  area </t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">absolutely beautiful and very good hotel cannot complain about anything staff are very friendly and helful specially mr shafiq fo always help and look after me breakfast was  really delicious inshallah i will come back again restaurant staff are also helful </t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i recently had the pleasure of staying at this hotel where mr shafikul served as the front desk manager i must say my experience at this hotel was greatly enhanced by his exceptional service and professional attitude his topnotch customer service skills professionalism and unwavering dedication to guest satisfaction made my stay at the hotel truly memorable </t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>i visited here several times i enjoyed staying here room and food is very good also hotel stuffs are very friendly specially mr bashar is a very humble person and i like his services overall i like ascot the residence very much and recommend other also thank you</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>wonderful experiences with the ascott hotel dhaka  restaurant food is assom room was very net clean hotel check in  check out is procedure is verybprofessional hotel all staff is very friendly  help fullmr shafiqul is one of them im strongly recommended ascott hotel dhaka best hotel in dhaka city</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>absolutely beautiful and very relaxing cannot complain about anything very friendly and helpful all staff specially mr shafiq front office always help  look after mewe took the all inclusive deal so breakfast lunch and dinner was great in nabihah restaurant also sakura japanese restaurant hade a great a flover with us will highly reccommend to anyone</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>i stayed in ascott hotel dhaka for  days for business purpose location is very good near to masjid a lot if restaurant near by the room is big and clean and they have kitchen also big refregerator to keep the food good if you have long stay in dhaka i would like to give credit for staff in reception abdulla islam habib specially mention of mr shafiq he is a very gentleman and helpful person they very helpfull during i am check in and check out also my any kinds of service  i will not forget ascott hotel dhaka he is my first and forever frind in dhaka city thatks for all of you</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>i viited acott the residenec hotel by my company ihi very nice noable stayed very secutrity n s ty earm is nice decoradedservice stuff ell known personspeciallly mr basher give me very fell cmtablehie make coffee very nice</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">excellent property and very convenient front desk staff are extremely efficient pleasant and helpful property is clean and has a fantastic atmosphere overall i had a great experience with the atr dhaka staff was incredibly helpful especially shafiqul islamduty manager he was a veryprofessional  helpful and the amenities were great the room was wonderful clean and perfect to celebrate the desired occasion will be coming back again </t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>very cosy hotel staffs are very humble and nice especially mr bashar who takes care of you well   deluxe rooms are better than  star hotel maintenance can be improved accessible from airport</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">everything is good mr islam and the restaurant collegues are nice and servicial the food and the service are realy good the conditions of the hotel are clean and confortable we recommend the hotel tonother peolple </t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>im fully satisfied with your services included food quality is very good  hygenic the hotel decor is by far the nicest ive ever seen playful and stylish tasteful yet trendy it features cool blues and whites with metal trimhotel was very nit and cleanthe stuffs are also well behaved with us mrshafiq  mrabdullah reception and other receptionist was very helpful and provided me the best servicestheir commumication level is customer friendly</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i am fully satisfy the service of this hotel  the environment services and food quality are really good  me and my family can spend very good time in this hotel  and i am excited to come again in this hotel staff attitude and maner are really good specially shafiq  duty managerhe is a very professional and co cooperative </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>the restaurant at your hotel deserves a special mention the food was simply exquisite and the dining experience was nothing short of exceptional the variety of dishes offered and the impeccable service provided by the restaurant staff made each meal a delightful experience   furthermore i would like to commend mr bashar and the entire team for their remarkable dedication and attentiveness throughout my stay their warmth and professionalism made me feel welcome and wellcared for during my visit it is truly a testament to the outstanding quality of your staff and their commitment to providing an excellent guest experience   once again i would like to express my gratitude for the wonderful hospitality i experienced during my time at your hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the staff at the hotel are very welcoming warm and well mannered especially sonia and bashar at the restaurant the ones at the entrance and the front desk are also very welcoming i would very much like to come back the next time i am in dhaka </t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>tasty food excellent service yummy fried rice with spicy chili oil chicken salmon cooked perfect and delicious workers are very nice and helpful pudding very tasty with cherry on top mr bashar very helpful with out table</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>good hotel located in baridhara diplomatic zone  very safe and clean staffs are super helpful and friendly esp mr bashar at the restaurant and the bellboy whom i couldnt remember his name foods are good the portion is big but i think it is quite expensive and take long time to cook</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>ive traveled all over the world and stayed at the finest hotels including the aman resorts i have never experienced the incredible level of services that i received at the ascott residence in dhaka bangladesh every single staff member i have met has always had a smile on their face and has  gone out of their way to provide the very best service i have ever received the list of employees is who have gone out of their way to make sure my stay is exceptional are too many to list i wanted to mention the entire management team concierge staff restaurant staff and housekeeping staff who have all made my stay one that i will never forget special thank you to zannat mahmud mohammad sonia mozid habib mr bashar and everyone else at the ascott whose name i did not</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>bashar down in the cafe very kind and accommodating made me feel welcome  i needed help with so many things and he came through for me i love seeing him i have some dietary issues he has helped me out with</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>everything is good mr bashar and the restaurant collegues are nice and servicial the food and the service are realy good the conditions of the hotel are clean and confortable we recommend the hotel tonother peolple</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the services of this  hotel is very highly professional such as food venue security cleaning etc are very nice they have sufficient trained staff who are very caring the venue attendant mr bashars is very cooperative </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>i visited the ascott the residence dhaka with my dear colleges for the purpose of vat tax training of plan international bangladesh the environmental  and total arrangement of the hotel is too good and also secured mr bashar and his team serve a treamendous service also</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the place amaze me with full of energetic peoples always keen to help with positive mindset ambience is nice greenary around the venue gives us good timebashar vai is good person mr mehedi is very cordial we will defenately comeback </t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">excellent support by the ascott the residence and the meeting room is very organized mr basar also very cordail to dealings thp bangladesh pleased to your service next time referer other thank you </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i am first time visit ascott residence  hoteli am very happy with meeting venue at serenity banquet hall roof top i was  there seminar of industriall union orgopen space nice garden venue also well decorated all service stuff are provide  good service specially mr bashar  give us remarkable  service </t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>hotel is very exciting and hospitable your services person are very nice and so kindful your breakfast is also good and delicios so taht i like very much  think come back again your personel islam is very good people</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ascott residence dhaka the provide as food in our giz dhaka  office metting food is good mr basar give up spesal service assisthe take care event giz venuascott hotel the wass regularly support most off the event thank you mr    basar your good support </t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>i stayed days ascott residents dhakait was very nice hotelvery security n safety areasroom very nice decoratedi enjoyed buffet breakfastfood was execilentservice stuff was very carefullymr basher  give us mind blowing servicethanks to mr abu bakor</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>it was a pleasure staying at this brand new property which is  minutes walking from the mall ascott the residence  is a nice hotel with excellent food and service they offer complementary fruit chocolates and coffee in the room breakfast is good and you can choose indian continental etc also the restaurant is very good and reasonably priced overall the experience was brilliant and enjoyed or weekend getaway a lot i will definitely stay there again</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i stay ascott residences dhakavery comfortable room is very nice n enjoyable restaurant decorated wellgood food l enjoy breakfast service stuff very good specially i mentioned to mr basher he make me very easy </t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>your hotel premises and internal ambeiance is very homelynice  friendlyim very pleased by your hospitalitythe foods of your restaurent is very tasty like home madelot of thanks to the authorities  employeesmrbasher  others</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>ascott hotel veery goodvery nice placementdinnerlunchbreakfust all good i am satisfaction all food and all service very welli am happy and my team very satisfaction  tnq so much mr basar vi for ur survice</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wow what a delicious lunch we hadwe really love the ambience nicely table arrangement by the service teamlocation is safe and securefood was too good service team is cery helpful always supportive </t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>good as a training venue the food accommodation and customer service is very good mr bashar has provided a good service the area is very safe and everyone is very well behaved thank you for the hospitality</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i visited ascott hotel residence i i said here one night i am really pleased to be here and the service and the food was really excellent i found it very nice and and i was very please to meet with mr bashar and is very kind hospitality  </t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>this is located in dhaka city at baridhara diplomatic zone its really nice hotel i had stay couple of days i was  spand the good moments is the hotel when i will be back then i would like to stayspecially  thanks to front office stuffs mehedi  shafiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">recently stayed best place to stay particularly one staff member who made my stay truly unforgettable emon a true gentleman among hotel staff went for a coffee and gave the remarkable service master at making coffee and all displayed best professionalism  a true gem </t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>i recently had the pleasure of staying at ascott particularly one exceptional staff member who made my experience truly unforgettable ashiful emon a true gem among hotel staff went above and beyond to ensure that my needs were not only met but exceeded ashiful emon displayed remarkable professionalism and efficiency</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>nice hotel in dhaka city ascott the residence  near by international airport  there protocol and transport service is very good durning check in time concierge service was fantastic as well as front office they had friendly attitude and smalling  face of mahedi   shadman also restaurant service is good  food was delicious emon is a maintain the proper service to the guest</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>ascott the residence is good hotel in dhaka city stay with friends and family location is very safe place at baridhara deplomatic zone restaurant service so nice also food very delicious front office guy mahedi very smart to deal bashear and emon nice support to us</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i visited ascott hotel rasidenc under democracy international programe there was i meet many services people all are them verynice  specialy mr basher servic man taker care every thing mr emon made nice coffee </t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i am rofiq from cmsd we take a food service from ascott the residence dhaka they have well trained food service man we meet name bashar we happy to take service from ascott the residence they give us nice services </t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>i am coming here  frequently to attend  the democracy international training they really took care us from their heartfood is goodbanquet is widewe enjoyed our training time herethanks to mr bashar for his very kind and attentive service also other service people also very cordial to our needsi feel like home here the rooftop outlet is really chilling place</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>hotel ascott the resistance is very good to stay with family  there are employees are too general  familiar there  behaviour is good restaurant food so good location is very nice palace all are good to stay in hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>enjoyed pleasant stay and great guest experience  hotel staff are great kind  polite and very helpful special thanks to sonia for her kindness and caring  great location nice ambience comfortable room</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>it was great experience in that hotel  room service was good and aslo breakfast great fav and the pickup and drown service was available in that great experience in that hotel and the hotel staff mahedi and rashed great person and good behavior to stay with hat hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>i stayed many times at ascott the residence whenever i came i felt that it was my second home the staff is very cooperative and attentive the rooms were very clean and they always took care of my preferences</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>this is my third visit to ascott the residence dhaka when i arrived i was under the weather the staff looked after me with genuine care zannat at the front desk helped me get some medication and sonia in the restaurant made sure i ate well i hope to visit this hotel again</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>we stayed one night in ascott the residence dhaka and truly enjoyed the experience we stayed in a suite and found it wellappointed there were eight bottles of water and a plate of fresh fruit waiting for us there was coffee and tea in the kitchenette and the bathroom had all the products you would need comb toothbrush ample products the cable in the room was nice too there were movie news and sports channels in english my family and i watched some tennis listed to music on vh and caught a bit of a movie on hbo the bed was a bit hard but i have heard that that is normal in bangladesh the ample pillows and cold ac certainly made the sleeping overall very pleasant the breakfast that was included in our stay was yummy too there were typical western breakfast</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>nice place for meeting good hospitality  best food  the hotel lacation is really attactive very good location ensure the easy moving of the various location of dhaka city safety is very concern for me found safety here</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>i spent over a week at the ascott residence and was extremely pleased with my stay rooms are comfortable and clean the location is ideal if youre looking for peace and quiet after a hard days work theres always a little attention on the pillow before bedtime so lovely every employee is adorable and caring  from security guards to housekeepers and from reception to the restaurant thanks to all employees for their kindness  special mention for masud harun and mahedi  hoping to see you again one day</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the hotel is very comfortableroom interior is goodfood is delicious variety of options at buffet breakfastfood and beverage service team are so caring mrmehedi manage his team very wellwell trained they took care our every aspects </t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>this second time im coming in dhaka so im very interested all services are good people very friendly i can moving anywhere with relative ease with the means featured here and the food here is also quite suitable for me thank you my friend mr islam</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wonderful hotellocated in very quite area safe and secure i enjoyed my one week staybreakfast is good lots of local selection is therethanks restaurant associate mr masudbasharand othersthey took care our group with nice hospitality </t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>i stayed in ascott the residence for four nights in june  it was my nd visit to dhaka in general the hotel staff is friendly especially abdullah from the front office dept the room is clean and comfortable</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it was best tour ever from democracy international the hospitality of this hotel is best in city i would recommend to visit anyone who are seeking warm hospitality specially i would like to mention mrandullahshafiqul and osman for their extra ordinary service </t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>it was my first time visit in bangladesh  and im so much happy that i booked at ascott the residence  everyone is so much helpful from front office they are particularly warm hospitable at their service specially mrabdullah it was such a nice stay  from the first day to last day i really appreciate for everything definitely ill make a plan for visit again</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the hotel is great and has wonderfull staff they accomodate requests and are very considerate and helpful rooms were clean and well maintained there is just the right amount of furnishing and good quality bedding </t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>the staff is amazing hit up islam hes awesome and cares about his guests good food and good coffee and fresh food the staff really cares about your well being and is always available to help this is a must visit site you will not be disappointed</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>very good service  abdullah alfahat is very helpful and cooperative housekeeping is very good as they asked for evening room cleaning  need toincrease the indian vegetrian food options so that will be helpful for guests</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>the room is very nice and comfy and i had a good hospitality by the hotel staff kudos to mr mahedi for keeping us checking in and checking out very smooth   the location is strategic and lots of food</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>good services and nice room hotel personnels are friendly and polite this time i was stayed overnight on my birthday hotel staffs are surprised me with the beautiful and tasty chocolate cake on my checkout date after i finished my breakfast  i really feel thankful for the big surprise and made me feel special  wonderful on my birthday i am surely to stay and recommend my colleagues for this hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>visited there a few days back simply in one word their service is outstanding the atmosphere of the lobby and restaurant is very nice they have a salon at the top of the hotel the staff are well trained and very supportive and cooperative</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>mahedi service guy is very good man he ready to help in everything you are requested  hotel provided complimentary and transportation to airport and downtown just informed them in advance feel safe and comfortable</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>good hotel to stay in dhaka room clean and comfortable beautiful menu and very good food staffs is friendly and supportfully very good service and safe to stay good place for you guy to stay mahedi and rashed are very good and friendly helpfull and support me somuch</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hotel staff are so friendly and cooperative from the beginning to end my experience was so good from the online booking airport protocol manager mr shafiq restaurant manager ms sonia front desk staff and even drivers all know good hospitality rooms are neat and clean breakfast is upto the mark thanks to zannat to help me on online booking  really it was great pleasure  to stay </t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>have visited overthere in this month with my partnervery nice hotel located in calm quite areabudget friendly and family friendly aswellfood and beverage service staff are very friendly well manneredwill visit again in future also</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>nice hotel the staff are super friendly they give me a lot of helps and advice during stays cozy room there are good services to pick up and transfer to the airport event in very late time  will be back next time</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>their service  food is very good i highly recommend this place the cuppacino is one of best in dhaka citytheir staffs are very cooperative and attentive to their guesti will try to come again to test their delicious food</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>true bangladeshi hospitality the rooms are clean the breakfast is good and the room service is extremely satisfying the staff are always smiling islam and jashan are very professional and greet you every time they see you the only problem is mosquitoes dont forget the mosquitoe repellent</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ascott residence has excellent staff and food sonia romana and masood are warm welcoming and attentive to every need all the staff at the hotel from restaurant to housekeeping are lovely id recommend this hotel </t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>great atmosphere and great service i was skeptical at first but they provided patience and understanding to every whim you have the location is great and very quiet with a home away from home feel if you need to stay in the diplomatic zone this is the hotel for you</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it was fine housekeeping needs some improvements room is clean and with basic items staff is friendly and helpful restaurant staff is attentive food quality is above average price is reasonableneighbourhood is safe </t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>friendly and very helpfull staf good place to stay food at the restaurant was good and cater to all needs breakfast had a good variety had a great time staying there located in a clean and safe area</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>mr tarik and his team made me feel at home from the start i always enjoyed walking from my residents through the lush residential streets to their hotel where i often dined a friendly and authentic staff with undoubtably the best coffee in dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the staff is very welcoming hospitable and friendly mr tarik made me feel right at home mr tarik is actively engaged with guests and ensures their comfort i extend a personal thank you to mr tarik and a genuine appreciation for the entire staff </t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">we love the hospitality here it was an short stay but a moemoral ones the people here were good with their services and special thanks to hasain sakib and mahedi for their support  and friendliness along the stay </t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">kind staffs clean room and quiet location it takes min to gulshan on foot also ride rikisha as well restaurants around the hotel are few but i ordered delivery apps pathao  i will back to here again </t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">very hospitable well furnished rooms the staff were very friendly and accommodating i have absolutely no complaints albeit location can prove to be a bit of a problem in terms of finding atms transport etc </t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>excellent hotel and i will definitely stay again they serve good food drinks hospitality of all staffs if you visit dhaka i strongly recommend to stay the ascott residence i can also recommend another group hotel ascott palace</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>good atmosphere with a good variety of choices in breakfast buffet the room interior is nice cozy and clean also a lot of thanks to the friendly greetings and services from mr mahedi as well as all ther other staff members</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ascott hotel one of my favorite hotel in bangladesh  i was visited with my wife for lunch  the quality of food and service was really good  mr hasan was serve us he is super star  also mr harun   mr g m mosharraf hossain khoka is he running this hotel been long time he is good human and idol for bangladesh  hotel industry  thank you mr khoka  </t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>the hotel staff greeted me with smiles and delicious mango juice but its a bit too sweet so id like soda if possible i feel safe because the security staff of the hotel properly inspects my luggage it would have been better if the hotel had a bar where you could drink alcohol</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>very nice experience  great staff and good vibes hotel is nice location  rooms are good and service was good rooms were what was needed for a business trip breakfast was fine good experience in dhaka very friendly staff as well as being very service oriented</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>excellent hotel very efficient and clean zanjar sonia and all the staff knew their jobs pick up at airport works well leave plenty of time to get to the airport as traffic can be very bad unfortunately there is not much to do at the airport if you are early</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>ascott the residence is nice clean and the staff very friendly and accommodating i had a pleasant and productive visit and intend on staying in the future i came in for three days to explore dhaka as a tourist but also had to checkin regularly for work i found the internet fast and reliable and i had no issue getting things done while my knowledge of the city isnt deep i cant imagine a better location than ascotts it is quiet and uncrowded but still close to the center highly recommended for either tourism or business purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>after finding other hotels fully booked due to postcovid booming i reluctantly stayed at this hotel for about two weeks however i feel that the management has changed significantly since before the pandemic and that the basic training for hotel staff is insufficient i was disturbed during my stay by instances such as staff loudly calling out names in the restaurant and the unstable internet connection resulting in repeated knocking on my door and phone calls asking if everything was okay after i had made a complaint three hours prior the lack of basic training for hotel employees greatly affected my sleep quality choosing another hotel would provide a more secure and comfortable stay</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">all the teams is good working everything care with me good communicationsafisfy with the internet connection good food good house keeping </t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>i would like to complements all of your staff being very professional with smile thier faceshave been very impressive in thier servicesi would like to visit again specially like to mention some staff names  ms sonia mr masud mr mahmudul hasan house keeping</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>the service was excellent with respect to all areas by zannat hassan and habib in reception shawan in airport transfers and restaurant i recommend this hotel quite highly for service with a smile throughout my stay</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>feel like back home again good service mind and taking care very well from mr mahedi and all the crew very good test for the food especially option number  with sweet and sour soup room also clean</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>here is quiet good as foods and drinks nice all receptionist is very friendly i have good support from abdulla when i have issued transport from hotel to airport it is traffic jam i worry late my flight</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>this is very good hotel hmm when i was last time stay was very good also food are nice today airport potocal service was fine and check in is nice mr sakib very good person also mr mahedi is very fast to come to room and mention everything and all number</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">very good services very good crew specially for  mrislam  good attitudegood foodgood handling from reception crew  good attitude from restaurant crew good support from the drivers  keep the good work up </t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>this hotel is very  nice  good everybody behaviour is really fantastic  bellboy mahedi is very smart to chuck in also description about hotel  room  security are also fine to security all everything  thanks for service</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>the hotel staff was attentive and very helpful particularly zannat at the front desk who made gracious efforts to provide timely and pertinent assistance the rooms are ample neat and cozy and the hotel location is unbeatable i would recommend a stay at the ascott for whomever is visiting dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the hotel was very well situated the staff were very friendly and welcoming mr mahedi and ms jannat was very helpful to us and provided ample attention and support for us and our guests overall very happy </t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>the hotel is just nice and clean as the expectation the service is also great would be a nice place to rest or during bussiness mahedi and abdullha are so cool serving when arrive alot of supporting just you can ask for the help here</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>very very good mahadi san he is a bellboy is so kind that he explain me many service of the hotel they politely explained which services cost money and which were free i would like to come to this hotel again</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>clean rooms delicious food and excellent service they had a wide spread of selections for breakfast lunch and dinner their welcome juice was tasty too shout out to abdullah shakib and islam  for their  star services</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">great service good food  many choices  good vibes peaceful place surrounding comfort room friendly employee good service by the receptionist abdullah and bellboy islam keep up the good work </t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>front desk is very accommodating room services were very helpful the room is very clean and tidy the food were good different items were prepared appreciated the complimentary items that were provided great services</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>the service was excellent and i feel comfort to stay here always room service found excellent  mr mahedi behaviour was good enough and he was very cooperative i fully satisfy with his service and in future want to visit more</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>everyone was very hospitable and helpful breakfast is good and japanese seaweed rolls are available the rooms are spacious enough and have good internet speeds and the bathrooms have good hot water mr abdullah was also helpful during checkout the airport transfer service was smooth</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>though it was my first visit in dhaka i have found staff was very cooperative specially mr  reaz he helped me lot regarding my laundryroom was very clean as well as food was very delicious i must recommend this hotel and i will inform to my company to accommodate me in my next travel once i back dhaka again</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>good serviced from andullah and teamdinner and breakfast  was great test and deliciouswe will back again and ascott hotel alway the bast for our team for transition and visit in dhaka bangladesh thank you</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>it is nice stay communication was good  would like to stay again when i visit bangladesh  thanks for mr abdullah and mr islam for better service breakfast was good i recommend to visit anyone who want to visit</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>mr abdullah and mr habib were really very helpful my stay was very nice people were always talking to me and asking how i was and if i slept well hotel location is good very accessible and good neighborhood truly a recommended hotel to anyone visiting dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>really nice stay room super cleaned friendly staff  emplacement of the hotel really convenient and all services available at the hotel with good service made me feel at home definitely recommend it</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>we stayed for  nights at ascott the residence in nov  having stayed at another nearby hotel right before moving to ascott ill have to say that ascott was excellent the room was beautiful with very clean sheets nice aircon and a great toilet more importantly the staff were all very friendly and professional from the security personnel and bellboy right up to the manager special shoutout to miss joanna for her kind assistance in making our stay a memorable one and habibur for excellent service and friendliness during breakfast</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">its very warm welcoming n staff is very helpful they help us in each n every way   specially sonia at the break fast desk  they really helped us with language issue which we were facing it very badly but the staff made it very smooth for us n guided us </t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>this is my st time staying here in over  years  but i will say these people remember you from airport collection to reservations to even mohammed ali he is the boy in restaurant   all a good crew  here  this was all in my  hours of being back here</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">stayed for a few days nice hotel in quiet surroundings in baridhara the room was clean and comfortable the staff was friendly and the service was good all in all i was satisfied and i would happily come back </t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>it was a good place to sleepvery relaxing placehave a good food also good serviceand good workerit is also have a good viewif you need something they can provide it to youto many food to choosekeep it good work</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>friendly staff makes my stay memorable one every time thanks to mr abdullah and mr islam sheik though i have no plan to back to dhaka at this moment i will surely stay at the ascott the residence next time</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>everything is good  from staff to hospitality cleanlinessthe quality of servicethe restaurant staff are very friendlythey make you feel so special  especially sonia  i stay there every time i visit dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>very good hospitally from zannat usman bhai and maruf and  the team members and i like to stay this hotel for the future recommended for tou stay in this hotel  i like the food and gym place also nice you can enjoy your karaoke time at night on  roof top</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best hospitality at ascott hotel dhaka appreciate welcome and take care at reception by senior staff name jannatthanks to jannat for wonderful hospitality hope to visit ascott hotel in next visit in november i am very happy and delighted </t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>we are confined to stay in only allowed hotels due to security purpose ascott is great choice among those  and i stayed more than two months staff are well trained and highly hospitality minded one thing missing is a small kitchen facility in the room for long staying guest</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>restaurant team are welcoming attentive and friendly every day a friendly greeting from sonia and team suite room is well provided with facilities hard to find in dhaka perfect for an extended stay baridhara is a quiet neighbourhood with parks and possible to walk around freely to the park small minimart or coffee shop</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>the staffs were super friendly especially to tarik sonia and hasan  recommend to stay here tarik was very professional and keen to help all the guest im very satisfied definitely come again for next trip  however the room can be improved the room need to be updated accordingly to modern facilities any other employees should be trained accordingly to international standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>very satisfied with the service from ascott palace management specially  bashar and jubayer was always therefore very well mannered and cooperative behavior food quality was upto the mark and as per requirement</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  a comfortable and quiet hotel with enough amenities equipped your requests and problems are promptly addressed  my stay was a bit long more than  month but my stay was quite comfortable there staff were friendly and helpful  mohhamad of the front desk sonia in the restaurant tarik officer and all other staff of front desk bellboy housekeeping restaurant security were willing to help my stay there great one i took some room services and the taste was nice</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>we had a pleasant time at ascott the residence i traveled to bangladesh with my husband and two children after a very long time i was concerned about safety mr md ibrahim reservation supervisor assured ascott the residence was a safe place to be and i felt very safe throughout our stay mr shafiq the airport protocol officer was patiently waiting for us when we arrived ms sonia greeted us every morning for breakfast and made sure we had everything we needed she packed bakery for us when we went for a trip and the day we were leaving because i missed breakfast it was delightful to see her every morning the staff abu bakor and habib were helpful overall every staff we met were very nice and made our stay comfortable we had the the business suite we really liked</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>i am staying in this hotel since last  month the staff is very friendly professional and always ready to assistthe rooms are clean and large with lovely decor and cushy bed that are pure white and so comfortable  food is very goodfreshtasty and healthyrestorant staff is very polite radiant and made me feel at home they have to improve laundry service because some time they not remove stains properly highly recommend this hotel if i came again this area i would like to stay here</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">had a great felling here  hospitality is on  next level feel like home here   all staff is very pleasant need to mention  some person which i interact more first is mr tarik and other is miss soniya pleasure meeting you both    lots of love from india  </t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>it was my first visit to dhaka and i stayed at the ascott hotel the best word to sum up my experience would be a fantastic hotel a everyone here is welltrained friendly and eager to do their best to meet our needs b the hotel is located in dhakas affluent region the diplomatic zone of baridhara in a calm and wellkept area that belies the image of the city you have in your mind c im also pleased with the restaurants food quality the staff and salman tarik bhai who also happens to be the coowner pr head tarik is a fantastic person and ive gained much knowledge about bangladesh and its culture from him i anticipate returning here once more</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>hi mahmud russel  it was nice time i had spent in your hotel stayed for  days so admirable polite humans from entrance to manager to service staff etc really your team is performing good mrrobin and captain were doing a great job i do visit again n again  spacious rooms hygienic and well maintained buffet superb  god bless you guys to serve more and more</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>i stayed in the hotel for more than a week the stay was great the staff was very warm and welcoming special thanks to mr tarik he is great in management and guest relations   the hotel is in prime location has good security and safe surroundings there are lakes gardens nearby for relaxing and jogging breakfast spread and food is also nice  overall it was a very good experience would recommend for family as well as business stays</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the place is comfortable the stuff is good sonia is a very nice employer always ready to help and support food is goodthe location is very good rooms are gooda good suggestion to stay when you come in business on the end of the day you can relax no noise and calm </t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>i have been staying at this hotel for about a month and everyone is friendly and very comfortable they try to remember the room numbers and food preferences of longstay guests and try to serve us comfortably when it comes to breakfast sonia and hasan in particular have been a great help to me every morning</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>stay at ascott was very warm staff are very courteous and the location of baridhara is just amazing and quiet spl mention of mr tariq he helped in all the hotel formalities and served with smile looking forward to travelling again there</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>great hotelgood support and service from staff thanks sonia and hasan for good services and all good delicious food hope to be back here again in the future who are looking for a good hotel i would recommend   here</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>room and people are good best place to stay during transit at baridhara area room are tidy food at restoran during breakfast are exelance room boy sheikh have good bahaviour fahad was a resiptionist has good personality</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>excellent hotel most friendly staff and best service   mr basher has been our host for the week and he has been doing his job full of passion we are most greatful to him and his collegues   also we enjoyed the dinner on the rooftop restaurant and the breakfast was delicious   we recommend this hotel to tourist and business people it is located in the most safe part of the town next to all the ambassies   family van haaren from the netherlands</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>good service all the time by all staff of the hotel and alway there to help the geust all situation of the guest really appreciated the crew of hotel from my side handoff all the hotel staff and front office</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>mr mahmudol hasan is a very warm sophisticated and able hospitality professional i recommend him very highly for hospitality especially room attending services his behavior punctuality and approach to work is very comfortable and effective</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>the staff are very friendly the premises are always very clean and well maintainedthe front office and all department are very supportive and especially mr fahad  are always looking out for the best for the guest</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>overall service was great very satisfied with the hospitali of the staffs specifically pleased with the service of ms sonia and mr habibur they were very efficient especially ms sonia was very warm and friendly an awesome experience so far</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>overall service was great very satisfied with the hospitality of the staffs specifically pleased with the service of mr abul bashar and mr abu bakor they were very efficient a great experience so far</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>as someone who comes to dhaka very often i found the perfect quite place to stay ascott residence in baridhara  road  i like this hotel because i feel not only safe here also relaxed and rejuvenated after spending a day in noisy and dusty dhaka coming back to ascott residence makes me feel like im in paradise similar to travellers coming across an oasis after a long journey in the desert clean rooms friendly staff which are always willing to help and assist and good quality food from many cuisines  i have stayed in many hotels in gulshan banani and baridhara and amongst all of them i would choose ascott residence it has the best dollar value</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>today we chose the special menu seafood plate at the hotel restaurant the food was very tasty the guidance and service provided by the support staff mohammad ali and ana emon was excellent thank you for your continued support during our stay at the hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>a quiet cheerful place sonia in the dining room was fantastic as were all the folks at the front desk the neighborhood is walkable and the rooftop terrace is serene very glad i stayed here for four days i would come back to ascott the residence in a heartbeat</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>everything is smooth every day newspaper is provided it is vey comfortable i enjoyed nice airport shuttle service i will come back again thank you  mr tarik sometimes i enjoy room upgrade for free</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>wonderful ambiance friendly staff beautiful rooms it was truly a pleasure to stay at the ascott residence and i would highly recommend this hotel to other business travellers i will definitely return here in the future thank you</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>excellent hotel with excellent hospitality by  front office dept  specially fahad behivors is amazing and all servive is good restaurant and food is good thanks for all  regards  jan fredrik pattikawa</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>undoubtedly a place where i love to stay while staying in dhaka let it be my business trip or personal one the restaurant guys serves the exact one which is asked while the behavior allows to feel cozy and experience the best suited place for me</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>very clean room and friendly staff breakfast was also very nice they allowed staying us until we move to the airport with free of charge thank you mahmud definitely stay again location is also good</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>experienced good stay with respectable staff  i selected this hotel after visiting  hotels in dhaka and tested  hotels in the country this is the best with comparison with the price  the location is good calm and suitable especially for those are working with embassies as it is in same area  especial thanks to sonia  nipune as managing the restaurant perfectly and for beautiful given flower but everybody tried their best for me to enjoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">all hotel staff are friendly and helpfully  breakfasts menu is always fresh  room is big and clean with more than  tv channel   that location is in barridhara so close to the jamuna shoping mall and my office at ghulsan area </t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>bourique style hotel with friendly staff and nice clean and silent rooms located in secluded and calm baridhara diplomat district and close to airport and downtown perfect three day stay in busy dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>the ascott hotel is a good option for any kind of traveler  and staff is very nice and helpful thank you so much for mr robin at front desk to be very efficient and friendly and also for mr sohagh for all the time being friendly and also helping carrying the luggage i strongly recommend ascott</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>it is surprising to find such a hotel in busy crowded city of dhaka to find such a safe and environment friendly hotel to enjoy restful stay and eat at well desirable restaurant  where you are served with great care  very good staff  basher arfan emon</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">this place is a gemfrom the receptionist to all the staffsthey were very friendly that we felt definitely at homemr harun from fb royal treat will always make sure our babys food is also ready for dine in everydaymr anwar from housekeeping dept was very helpful in making sure our room is always clean and special thanks to mr habibur from concierge for taking care of all our belonging and definitely to ms zannat our beloved receptionistshe helped me a lot during my stay herethese experiences are truly memorable for us whole family and we will definitely visit this place again  </t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>i fill comfortable and they are service is good enough all the staff always served with  a smiley face the recipe offered by them for guest are healthy they try to meet the customer requirement even try their level best</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>ascott the residence is a nice quiet and clean hotel the service is excellent mr basher and mr shahadad were extremely helpful throughout my stay would definitely recommend to guests travelling to dhaka bangladesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>every time i visited ascott it feels like partly arriving home the staff is welcoming especially sonia gives big effort to make me happy the rooms are clean and spacious there are plenty of international food options in the menu of the restaurant and most of them have decent taste highly recommended</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>they were able to meet my various requests including extending my stay during the first part of our stay breakfast was on order every day due to covid when i stayed there in june this year they served mangoes for breakfast which was delicious but i was little disappointed that there were no mangoes this time</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>the hotel staff was so kind to me especially sonia mahbub and zannet this was the first time to visit bangladesh so i didnt know enough information like foods coffee stores they kindly told me about it and those were really nice again thank you so much for your support and giving me special milk tea as well</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>it was nice to stay here with great hospitality and service they are good at hospitality food serving at room and continuous takibg care behavior was good from restaurant they were also good at food serving keep goes on like this</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>in entering the hotel looks quite ok but only to go to the restroom shows exact what is the standards here staff members are not paying attention to new guests only frequent people the food is not very good at the restaurant and served cold and underdone i asked to speak to the cook but was told he left early no manager around only a suoerviser not professional at all meeting room very dark and not clean</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>i frequently visit ascott the residence for family visit as well for business i would like to say that i have found mr tuhin mollah always dedicated for his work he is wellmanered knows wht hia jib is very well i wish him all the best</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>safe location adequate amenities great staffs and service heheh no sale of liquor though rates are reasonable high marks for hospitality among others had a light conversation with a staff named tuhin</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>really a nice stay the restaurant host ms dewan and the staff is always ready to help you out with your needs different kinds of foods for asian regions gives you the choice of try different things every single day   recommended</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>its a satisfied experience staying in ascott the resedence the behaviour of the staff are really careful and respectful especially mohammed monir uddingro is the very good personi come back again in this hitel</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>it had been a good stay the staff were hospitable including housekeeping mr harun and he had made my stay comfortable everything was good there the food which had come to my room and all the services was great</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>i am satisfied experience in staying in ascott the residence mr md ruhul amin the dinner and breakfast orders are customizing as per my requirements and mr harun the housekeeping person is done a good job while cleaning</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>i spent  days here on businessi must say that everything was excellentthe room is very comfortable good services good  house keeping thanks for mrharun he did the good job  i would recommend this hotel to other having a business trip</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>i stayed this hotel for couple of days for business tour their services were good specially their support staff behavior they always tries to meet the user expectation as an example i requested for customize dinner in couple days  they tried to manage the foods accordingly</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it a satisfied experience staying in ascott the residence the behaviour of the staffs are really cheerful  respectful the environment is safe and sound happy to be a part of it hope we will meet again best wishes </t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>it was a great experience the place was so good as well as the foodservicewe are highly pleased with the behaviour of stuffs and their services  specially sonia tuhin  and  mahmudul they are so good at their services we  highly recommended ascott the residence</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>overall service is so so but hotel view isnt that much fascinating even the hotel doesnt have a proper gate to recognize from outside service people are cooperative  as well as their restaurant peoples thats  a positive side</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>truly appreciate your team support  service  hospitality got during my time in ascott the residence i believe everyone will feel same comfort here or even better you guys are amazing good luck</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>in  i stayed six months in ascott residence in dhaka  under covid crisis mrnayeen and his team garantied all guests helth security permanently h meanwhile i could stay safe and feel protected from any risk during my stay in your hotel moreover i recognised that it is quiet difficult to keep service level under such a sensitive situation that is reason why i really appreciated your efforts and professional attitude in service under such a situation off course i sould not forget to menton meal quality of break fast lunch and dinner in ground floor thank you very much for your efforts good luck for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>after about  years not coming to dhaka this year during covid pandemic i need come over to dhaka again for work this year prior go to location need to have  x negative covid test ascott residence have good staff all of them are kindly to help you you room cleaning everyday mr rupon das such a kind staff room boy that clean my room perfectly good and recommended hotel to stay one more you will get good food during your stay</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>i have stayed ascott from  june to  july all of staffs are cheerful and cooperative to our work i really feel gratitude for them and this first trip to dhaka should be great memory namu shinnyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>i stayed about  days in ascott residence hotel facility is a little old however house keeping is very good so i could stay comfortably especially my room service staff mr suicongon and mr ahumdol are very kind service for me thank you very much</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>its great service from hotel the staff are friendly and always care about me if i have any problems thank you mrrupon das for taking good care of everything i am very impressed and will stay again</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>i stay here in asscott the residence dhaka for five days  i have found there hospitality and food was good staff were very cooperative and helpfull i am satisfied about there behaviour overall services was good thanks to ruhul sonia  rupom for your care</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>really a pleasure stay in this hotel while all the staff guided and followed by strick covid protocol during my  day stay in this hotel have found all the staff from dining to housekeeping are so much engaged to served with best to his guest i have meet mr rupon das as housekeeping staff and really amazed to his nice and polite behaviour with all his experience and dealing with his guest  food was really good and during covid all food served in individual room with maintaining high level of sanitizing food price need to review as some of the item looks so expensive considering the item itself  happy staying</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">this is the nd business trip in dhaka japanese feel anxious about traveling to dhaka at first because dhaka and bangladesh are not very familiar due to their long distance but this hotel provides great hospitality and satisfies many japanese the room is kept clean every day by nice house keepingroom attendant including harun who is in charge of my room this time hot shower and bathe can be enjoyed every day which is beneficial for japanese as well the restaurant food is also good though the limited kinds of dishes in breakfast and uneven taste sometimes disappoint me however tania a nice cooker in the restaurant cooks very well and her soup is excellent for most japanese  </t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>this is the rd visit in ascott the residence dhaka  ive received daily service from mr rupon one of the housekeeper in this hotel he accepts all my requests and very eager to give me hospitalities every day</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">this hotel is cleaned up my housekeeping person mr rupon das is always cleaning my room every day very hard so that i lead comfortable business travel days  here </t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>good place to stay with very supportive and decent service team comfortable arrangement and restaurant service  special thanks to tuhin  ruhul and tasfia for your warm hospitality  appreciate your efforts</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>sonia and her team is excellent sumsouzzaman dewan is best person i got nice attitude and services from them hotel is a good one food and other services are ok food service at room is neat and clean</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>it was really nice hotel in dhaka especially its room service and house keeping the taste of the meals were good but it took  to  minutes for the room service mr rupon was really helpful for keep the room clean during my stay in the hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>during my stay at hotel ascott residence from  june  i found housekeeping assistant mr rupon das helpful  enthusiastic for delivering world class service im wishing good luck for this smart guy so that he will continue delivering his best  saifullah limon chevron bangladesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>place is very cool and calm they improved their food quality especially for bangladeshi people for their more improvement they should change their room furniture  furniture are old fashioned and looked dirty their room service is very good especially mahamudul hasan was very professional and decent hope their future success</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>its good services from the hotel they improved their service from past  specially room service by rupon das a very helpful and coordial person to serve ascott improves its food quality also this time i am very much happy to stay here</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>the staff are friendly and always care about me if i have any problems in fact when i told the receptionist that i wanted to use the microwave oven in the room they came to set it up later that day life in bangladesh is difficult for japanese people but the hospitality delicious bengali meals and hot baths make it a good place to relax for a long stay there is also a small supermarket on the road next to one and japanese cup ramen and pocari sweat are also available so you may feel safe when you are homesick   thank you very much to mr rupon who works like my concierge</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>for business i have stayed here  months all staff is too much kindness and try to their best for us staying comfortable especially mrrupon das housekeeping staff and mrmorra and mssonia restaurant staff thanks for about helping my some troubles and working hard allah hafis</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>i stayed in this hotel  days during my mandatory institutional quarantine period everybody was very helpful friendly and professional it is hard balance these especially sonia in the restaurant make feel like special guest and all kitchen staff tried to do their best to accommodate my needs definitely will come back</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>i have stayed at this hotel for over a month it was so comfortable that i didnt want to leave during my stay i was lonely on my birthday but the hotel staff seemed to be aware of it so i received a surprise present with a cake i was very happy with their concern all the staff are kind friendly and polite thanks to that i had a very good time they responded promptly and politely in the event of some trouble such as the noise of neighbors or the lack of internet access and all the food in the restaurant is delicious especially the shrimp dopiaza is the best if you ask for breakfast it will brew a very delicious cappuccino this hotel is just like my hometown in dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>hotel staff  facility are good i enjoyed my stay   decent hygienic and covid safety measures in place   i stayed there for business purpose overall hospitality was great   the location of the hotel is the most secured and quiet placed</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>hotel ascott the residence check in  mar  check out  mar  room no    unparallel services for which i recommend ascott  restaurant incharge sonias sincerity efficiency responsibility  punctuality  special dishes chef kilpots taki fish mash vorta  excellent room service especially hasan tuhin bayjid  tanvir  i heartily remember mr sizar who was very amiable and professional but is not currently working with this hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>been there for five days and has a awesome experience regarding most of the service they provided the staffs are really friendly and service delay is minimal while the food was also good when you choose for traditional items have little mosquito issue but after aerosol spray its okay</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>excellent service and covid safety measures in place the best of the best is staffs behaviors professionalism and remarkable communication skill i stayed there for more than  days due to business purpose and found cleanliness timely food and laundry services the overall hospitality was great and special thanks to mr harun and mrs sonia for their professionalism the location of the hotel is the most secured and quiet placed in the busiest dhaka city recommended</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>i have been staying in ascott the residence for several times during this pandemic situation due to business purposes i must say they have shown thoughtfulness in terms of hospitality room services and cleanliness mr ceaser and ms sonia were very proactive in ensuring all my requirements during my stay   nevertheless they have some improvement opportunities in terms of food preparation i felt that the food menu could have been more versatile  overall i am pleased with their service and hospitality  recommended</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>i stayed here for couple of days n the service was quite impressive hospitalityfoodprompt response to any problemcordiality everything was so amazing that i started feeling at home i must mention about mrnobel from restaurant team  mrreaz from reception team who were too supportive thoroughout my stay here as i got sick during my post covid duty isolation periodthey managed drugs immediately for me  adjusted menu according to my taste  the hotel is clean  offers a good view also</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>excellent service and all staff are very much cordial especially front desk officer mr mahfuz he was very good person and friendly personally i think i like him very much also best service provider in this hotel highly recommended to visit ascott hotel if you are in short trip or business work good environment nice place for workoutspa and other facilities are available location was perfect and its a feeling like i was out of dhaka it was almost noise free hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>the hotel is clean and provides great hospitality  the front desk service provideer mrrobin is very much gentle and a very good guyhis behaviour was awasome  the restaurant and room service provider mrnobelhe is best in resturant and room servicemrtuhin and a womanname cant rememberis very helpful  the housekeeping and room cleaning service provider boys are really greatthey always fulfilled our dimand or any need  the other staffs specially mrsohag were very helpful the car drivers were also good the hotel provided me almost every facilities  the rooftop cafeteria and gym of hotel was great  overall experience was awesome  ill recommend this hotel to every couple and families</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>i left ascott the residencedhaka yesterdayi stayed there for weeks for my covid duties in bsmmurooms were well decorated cleanhouse keeping service was good especially i would like to mention tania she was very helpfulrestaurent service was okall were very helpful for us especially mrnobel of restaurant all services were satisfactory but one thing i must mention that food seletionmenu was not so goodit should be more tasty especially the vegetables with onion was  undercookedfried rice was tasty but the vegetable curry chicken curry was not good rather fried chicken was gooddesserts were tasty especially pudding  payesi enjoyed all security service was excellent i enjoyed my quarantine period happilythanks for your hospitalitywish u all the best</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>located just near the us embassiperfect location  the hotel is clean and provides u great hospitality  the restaurant and room service provider  mrnobel is very helpful and will guide u throughout your stay  the staffs were very helpful the hotel provides u almost every facilities  the rooftop cafeteria and gym of hotel was greati mean it   overall experience was awesome  ill recommend this hotel to every couple and families   you wont regretjust be there</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>tomorrow i will leave this hotel i have stayed here for  weeks  i am fully satisfied with their services all the staffs are very cooperative foods are tasty room is well decorated and clean among all the staffs i specially want to mention mr hasan mr surongon of housekeeping department and mr nobel of restaurant they know their jobs best i wish to visit here again</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>location of this hotel at diplomatic area very calm and quiet region of dhaka they have well mannered and well behaved staff all are sincere and responsible to service room are well equipped and modern facilities present food are also food</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>excellent service highly recommended if you are in short trip or business work good environment love the foods nice place for workout and guess what spa and other facilities the surrounding security is also fantastic</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>service and food is satisfactoryfood was goodhouse keeping was timely and satisfactorythere was  complementary laundry each day hotel room was beautiful and comfortable alsothere is a beautiful roof top location was perfect and its a feeling like i was out of dhaka it was almost noise freebut gym need a bit maintainanceall service men were friendlyover all i am satisfied and recommend it for visitors</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>we visited the hotel to stay away from our family during covid duty the service here is excellent all the staffs are very much cooperativeamong them i can name mr mahfuz mr motin mr mahmudul and the food was excellent  if u have any discomfort u have to just ask the authorities and ur wish is granted moreover they served a birthday cake for one of our colleague during our stay and it was complimentary  i wish this hotel all the best and surely recommend it to u all</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>all staff are very much cordial epeially tania and novelfoods are are so much delicious and desert are awesom  especial thanks for for my birthday cake which are so much testythey maintain proper hygiene in that pandemic</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>i was visited for business purposeswhen i entered the hotel i looked staffs of this hotel are all friendlythe front desk officers are very accommodating and so kind basically mrmahfuz was excellent security and bell boy are also good the restaurant staff are all very pleasant and friendlyfood was excellentwhen i free i will visit this place again</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>the location was great for my offices the rooms are very clean and functional i loved the different teas the staff were superb especially sarowar on the door who was like my brother during my stay the restaurant has something different everyday and the chef offered to prepare british food if i was homesick</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>the staff of this hotel are all courteous and friendly the front desk officers are very accommodating and they remember you by name and your your needs the restaurant staff are all very pleasant and friendly especially sonia and gloria</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>writing this during the pandemic not sure when i can visit the hotel again we stayed in mid march and i wanted to say a word of appreciation for farhad in the front desk who used to give us travel tips hope i can stay in the hotel sometime in the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>the staff of this hotel are all courteous and friendly  the front desk  officers are very accommodating  and they remember you by name and your your needs  the restaurant staff are all very pleasant and friendly especially sonia and gloria</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>sonia in the resturant was very kind and cheerful  she made the breakfast more enjoyable  her enthusiasm and professionalism to serve and guests make guests comfortable etc were manifest each time i visited the restaurant  it made me welcomed and gave the place a more familiar and my place kind of feeling the guest room had a strange lowfrequency humming noise in some locations but not the other  for example youd notice that hum on one side of the bed but if you move the head to the other edge of the bed it becomes almost inaudible  it was the loudest where id sit and work on pc at the desk  it persisted when ac was off and sometimes it stopped and restarted  no idea   two other problems the bath room has a mechanical ventilation fan installed in a small</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>spending time at ascott restaurant is amazing especially when tuhin masud sonia and harun are around my mind still reflects their big smiles and treat would love to come to the hotel and enjoy the services again and again you all keep up a good job</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>the ascott is very good and clean the restaurant has an extesnive menu and bashir and sonia will look after you well also sarowar on the door will become your good friend highly recommended the ascott is a home from home</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">this hotel is located in embassy area and is more safer for foreigners and hospitality is pretty awesome especially ms gloria  mr bashar at the restaurent was so co operative along with the other staff  thanks to ascott team for a comfortable stay </t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>after my trip in bangladesh working as a nursing instructor in tangail this space was the perfect place for me to replenish my self i liked the massage i got especially and the food and the service in the restaurant were impeccable i highly recommend btw i am so delayed to write this i was there last winter in  and i am finally sitting down to write my review sorry sonya for the delay</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the hotel was booked through my admin team i find it nice and the hospitality is so nice so like to address from the airport starting at early morning  am till now the service is outstanding  the way they treat people with a big smile and take care of you where you dont feel you are in a hotel  few days missed breakfast but its was nice experience with dinner overall the food experience was great naming few by name gloria the smart breakfast person bhasar and the whole team working on was great tuhin smile makes my day more enjoyable  the missing part is the spa and the gym my bad luck both are under maintenance   </t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>locates in a very safe zone of the city room is big highquality towels good hospitality of staffs average breakfast   beware of mosquito  not just in the hotel room but in general of dhaka city</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the room rate is bit pricy as there is no room for selection around the town since the  terror attack   i was not satisfied with the associates naming customer with such a loud voice form morning till late since they were trained in that way but i would request to the hotel managers to ask him her not calling my name all the time in the public room is pricy and the facility shall be updated particularly the health gtym   </t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>me and my wife recently stayed at ascott the residence for a longer period and were nothing else but very pleased an incredibly friendly staff all the way from general manager to housekeepers we always felt at home   the restaurants provided great food for dinner as well as an excellent breakfast that was even further improved our last week there and we were always happy to have a chat with the staff while we were there   we cannot other than warmly recommend everyone to come here</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>i stayed at ascott residence for three months for my business trip it was my first time in bangladesh but the staff at ascott residence did everything they could to make me feel welcome the hospitality of this hotel is amazing special thanks to the staff at the restaurants and the concierge who greeted us and talked to us everyday  would come back again</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">every person is so kind and special for guest in my staying there were not any problems just one point id like to request to install baralcohol service  and if we can have a pool  it be perfect </t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>the environment is very great and the staffs are very friendly located in peaceful environment the hospitality is at its par lovely place for short or even long trip will recommend to choose ascott for your visit</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>placed in a very safe and secured zone friendly enough with professionalism the accommodation the food the amenities are simply great most importantly the service we have been provided is good enough</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>very nice hotel with comfortable rooms and facilities very clean and hygienic good food and especially great coffee great for business travel in a safe part of dhaka the staff are outstanding in all areas</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>there food service was great the atmosphere was too good specially rooftopbehavior of all the staff is excellent overall the service was great we are satisfied with their service a good experience with them</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>this accommodation is placed in safety area and suitable for business trip for foreigners every facilities are clean and neat and clerks are so kind if you come to bangladesh i recommend you to stay here</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>ascott is the hotel i very often stay when i come to dhaka it is located in a safe district and the service provided by hotel staff is comfortable they were kind enough to support anything she needed when my friend injured her leg</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>i spent nine consecutive working days at the hotel as part of a work commitment the hotel is located in the oasis of the leafy diplomatic district i was not an inhouse guest but i used the hotel facilities and had a delicious lunch there every daythe team does a wonderful job in making guests feel welcome including remembering names and how you like your coffee and the food in the restaurant was always fresh and tasty all the staff i met were great but sonia was a standout thank you for a memorable experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>i stayed one night at ascott on my way to berlin to attend a theater festival as a guest of the goethe institute and i was pleasantly surprised to discover this nice little hotel offering top quality service and amenities strongly recommend for others and wish the owner and management of this classy hotel good luck</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>having completed a successful training sessionthe environment is good enough  the service alsothey are so humblemost importantly their staffs have made my program incrediblemr tuhin  mrs farzana contributed a lot to carry out our training conveniently in an efficient waythey r very fast at service as well as polite alsotheir service have made me feel honouredthey have served to all our trainee timely and ensured the best servicethey have always handled all the tiny problems patiently  gave us a no problem vibesmoreover it was a great meeting in this hotel with these well behavioral staffshope will be there again to grab their most comfortable services</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>as a frequent traveler to dhaka i usually stay at ascott the hotel is comfortable and meets most of my needs its nice that most of the staff has remembered my name as usual great service provided by team of mr jasim arfan delwer at the restaurant  keep up the good work</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>i stayed at the ascott for several days in may   super friendly staffalways a smile  the dining room staff are extraordinarily kind and pleasant even offering special ginger tea to help me recover from a cold  overall clean and quiet and very comfortable</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>very clean  organized safe and convenient  pleasure to stay at breakfast  and coffee is amazing and staff is very helpful they got my laundry done at amazing speed will definitely stay here again on my next trip</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">great  helpful staff but room had a very unusual smell  bed was extremely hard  i think that these can be improved i understand that the hotel is relatively old however i havent seen any mosquitoes or bedbugs so these are good </t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>i stayed there for the second time for around  days staff is extremely nice and helpful the location is very good the rooms are very good and clean and the breakfast is very yummy and with a lot of variety</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>ascott the residence is in the gulshan diplomatic area of dhaka in a quiet residential street close to several major embassies it is under the airport flight path but the noise was not too bad there is very little other than residential buildings within walking distance of the hotel apart from a convenience store in road  and another ascott hotel in road  as with most hotels in dhaka there are security guards at the entrance to the car park who screen your bags with an xray machine and at the front door who screen you with a metal detector the hotel is quite small but has two restaurants a gym and a spa the restaurants have a wide selection of good quality local asian and western meals but these are subject to a service charge and vat which adds significantly to the</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>the hotel is placed in quiet and residential area of dhaka the rooms have good sizes comfortable bed and good connectivity to the internet there are many places to have informal meetings with visitors and a terrace very pleasant terrace at the top floor the staff is very helpful and amiable i had a very nice second stay in this hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>all the services of the clerk is excellent the room is always clean i feel so comfortable whenever staying there the location is in the most safety zone in dhaka next time i decide to make reservation again</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>very good service any problem occurring is solved immediately in the suites there is also a little kitchen with micro oven electric stove and different utensils for making small dishes all channels available with  television</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my week at the ascott residence was very pleasant it is a great hotel with spacy and clean rooms friendly and helpful staff and a relaxing rooftop terrace where you can enjoy great coffee and the specialities of the japanese cuisine i would warmly recommend staying here if you are one a business trip or looking for a more quiet residency away from the hectic dhaka </t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>i stay here regularly during our frequent business trips we enjoyed dinner at chill n grill rooftop restaurant great service provided by ms farzana and food was cooked very nicely by chef tania keep up the good work</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>ive stayed at this hotel or its sister hotel  theee times now the service is wonderful all the staff are so friendly and helpful the place is very clean and the food delicious and does not make a uk tummy ill it has a superb coffee shop also which do good coffee and i admit im a dreadful coffee snob i highly recommend it</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>the ascott residence was a wonderful place for training in a quiet location in dhaka with excellent rooms wellbehaved and responsive staff variety of foods and others you can pay visit over there</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>the ascott residence was a great place to hold a training course for a week  in a quiet location in dhaka with excellent facilities the staff could not have been more helpful with mr bashar going to all lengths to ensure we had everything we needed and our week was a great success highly recommend</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>stayed in this hotel for two nights i really liked its attentive service fantastic food both restaurant on the ground floor and chill and grill bbq  terrace and location of this hotel i will definitely recommend this amazing place if you want to visit dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>thangks for your hospitality especially for the ebullient sonia the artistic coffee treats from ashish and warmhearted tuhin i remember your genuine smiles and your kindness i enjoy the tranquility here</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>stayed here for few days  very attentive service daily newspapersslippers complimentary fruit airport shuttle the restaurant staff remembering how we liked our coffee without asking the folllowing day all the hallmarks of a very good hotel that looks after its clientele  what i particularly liked was the fact that as a woman i felt safe spending here the final night alone without any concerns at all</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>i have stayed  nights in this hotel everybody was so amazing and the staff is very lovely everything is very standard jasim and sayed in the restaurant were really great people and served beyond my expectations the food was amazing and delicious and i enjoyed it the hotel location is really good and everything is in reasonable distance i recommend this amazing place if you want to visit dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>i have stayed at ascott the residence more than several time  i feel very safe and comfortable food is good with nice variety  i wish the gym on the rooftop has better equipment and more room with open view</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>very nice experience  stay at this hotel which makes you feel comfortable secure  gives you a taste of bangladesh hospitalityi really liked the fact that they care about small details such as a fruit platter in room on arrival  one small snickers bar after clean up is kept in the roomreally very nice business hotel which is very secure and provides excellent service</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>we stayed here for a week and were very impressed with the extremely diligent service and the kindness and friendliness of all the staff the rooms are very comfortable and clean and we appreciated the little touches such as mosquito spraying the room the chocolates and the newspapers the breakfast offer is very diverse and caters for all types  bashar and sonia deserve special praise for their hospitality and excellent service and always with a smile jacim also deserves a mention for his allround attentiveness and care  mohammed ali in the chill and grill restaurant provides good service</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>we often stay this hotel and bring drink our self staff prepare ice cube a lot at st floor restaurant ms farzana staff is very kind  shuttle bus service have every hour morning time they pick up and send airport</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>i stayed here for  weeks for work  friendly staff good service on our last night we had dinner at roof top restaurant  great service was provided by mr mohammad ali senior supervisor the sirloin steak was cooked to perfection by chef tania  i would recommend the restaurant</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>this was my first stay at ascott the residence and it was great the room was average with a very firm not soft mattress but kept spotlessly clean by the thoughtful housekeeping staff who left me complimentary fruit lined up my shoes and even left me a snickers bar at the nightly turndown service i think the evening staff members name was masmud but i didnt meet the daytime staff i had several meals in the restaurant which i was glad to see has many vegetarian options and the breakfast was great but the best part of the restaurant is its staff especially jasim and sarya who remembered my name and my drink preferences  they were fantastic and warm the hotel staff overall were very helpful and concerned to make sure i had a good visit to dhaka ill be back</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>stayed twice in this hotel over one week period room number  and another xx forgot the number  the first time i was upgraded to the luxury family room which was rather spacious the decor and design was a bit old fashioned with slight unpleasant but tolerable smell the smaller room which i stayed the second time was better  wifi connection throughout the stay was horrible inside my room constantly drop connection after    minutes  however i would applaud the staff there for creating a memorable experience for us specifically delwar and jasim of the fb service delwar was quite chatty and attentive they even gave us a surprise birthday celebration to my friend kudos to the staff of asccott the residence</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>all the staff of managers reservation officers receptionists bell staff security guards waiterswaitresses and chefs men and a lady of the restaurants on the ground and top floors room services fitness club receptionists technicians and drivers are well educated for hospitality of guests i stayed more than  days in total in the last  years on business and everytime i feel happy to stay with the staff off course i wiil be back</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>reasonable accommodation near deplomatic area with security breakfast was ok but much scope to improve options and varieties for vegetarians dinner also ok no public transport or other options not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>it was a pleasure to stay here excellent service from arrival to departure  staff is very professional friendly and helpful rooms are very clean with all amenities you may need the bed was kingsize and very comfortable for sleep   wifi works average speed  the hotel restaurant had a small buffet breakfast also provided a continental breakfast for the early departure the restaurants staff was so helpful  nice attitude  they offered food  taking care like brotherhood  specially mr jamal thank you so much for your excellent smiling service there is no swimming pool but so nice rooftop it is ideal hotel after a long flight i had a massage before departure it was also good and reasonably priced   the hotel is located in a very  safe  secure place  i would</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>this is my rd dhaka visit with same hotel and always staying here for almost  days  ascott the residence covers all the basic needs for the guests mostly business traveller and foreigner rooms are very clean comfortable the best part of this hotel is warm  friendly english speaking staffs  house keeping teams are really excellent and always stands with support towards your needs foods are superb and you may feel extra superb because of charming energetic fb team members they always at your side with their best quality foods all members of fb team including their managers access your requirements and serve you the best one of their team member namely ashis is simply superb personality energetic and sound knowledge about culture places foods of bangladesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>ascott the residence is the older of the two this group operates in this neighborhood i was told  i used to stay at the other property ascott palace and this was the first time at the residence  compared to palace the lobby at the residence is smaller and the restaurant darker  they are both functional but could use a new decor  very steep ramps at the entrance and between the lobby and the elevator level should be improved for better safety to those who are less strong or tired from long flights  the room is spacious the bed is hard and comfortable  large work desktop is good and the power outlets are in the right place  i had a problem with the ac  probably an ancient unit it was very loud and cannot be turned low on wind speed  well it goes into low but</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>though its premises is not so big but its hospitality is so nice and very secured for its location all the staffs are well mannered and hotel is well furnished with neat and clean rooftop is green with bbq facilities after all that we love it</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>i stayed there for  days for a workshop that took plce in the same venue both my stay and the workhop were simply excellent i would gladly return to this amazing hotel my highlight all the staff is incredible polite and always willing to help</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>ascott covers all the basics as a hotel whose guests are mostly business travelers from outside the country rooms are nice and comfortable decently clean and very good complimentary breakfast the best part of ascott is its warm and friendly staff everyone speaks english always ready to help and always makes me feel at home the wifi connection is a bit weak in the rooms other than that i always enjoy the famous bangladeshi hospitality i receive every time i stay at ascott</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>very good hotel with excellent service and very friendly staff hotel restaurant has very good food with hr service and the breakfast is excellent rooms are very clean although the view from my room was to another building under construction the spa and fitness centre is small and dark but the treatments are very good and excellent value for money the location of the hotel is near the airport and in a very secure area although a bit far away from shopping centers internet wifi is free and of very high quality overall a very enjoyable stay</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>the accommodation rate of dhaka city is higher than that of other countries this hotel is cost performance good also this hotel is not big but it is wellbalanced room that clean and wide  i am always relaxed thanks to the helpful and friendly staff</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in down town and safety location room very comfortable and good cleaning service restaurant on rooftop is a bb  managed by mr basher very professional person breakfast full of options for every customerincluding italians </t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>the hotel is doing its best to keep the guests as comfortable as possible during their stay friendly and helpful as it should be good breakfast and evening options available i will return when i am back in dhaka  ps i have a feeling they upgraded their internet</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>i enjoyed my stay at ascott mosahid helped me to change my roomenjoyed kind welcome every morning at the dining roomthank you for your smileashishiall the staff are very nicethank you all and see you again</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>stayed at the hotel for first and last parts of a trip to bangladesh  well appointed gracious staff comfortable in a quiet part of the city  airport pick up and drop off service much appreciated  nice to have a small work out facility  my favorite part however was breakfast  delicious expresso graciously made each morning by sonia and basher fresh yogurt and fruit</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>excellent guest relation thanks to mosahid for taking care of me so well he attended to all my requests with diligence had a memorable stay food was good room service was excellent excellent internet facility</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>it is a small place with good servicethe rooms are very bigyou dont feel suffocated instructions for using everything are very clearly mentionedit is very near to gulshan where all the shopping area and restaurants are located</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>though one of the reviewers is right in the sense that the property is a bit old it is well kept and maintained and the service staff are very professional and courteous every level of assistance was provided to make our stay more comfortable the food served at the indining facility was delicious i loved it the area is a quiet neighborhood well guarded as most embassies are located in the area and is clean and green even though i never did get the opportunity to walk around the area during my too short stay i would recommend a walk in the park just a few meters away just for the quaint scenery it provides i would have loved to myself  the toilets could use a bit more scrubbing though they were well cleaned in short loved the stay and i would recommend the place</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>perfect location safe area although quite boring excellent service staff are very nice and food at the restaurant is very good the gym could be improved excellent value for money but lets not forget that salaries in bangladesh are very low</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>i stayed here for two weeks and highly recommend the hotel and its staff  it is located in the quiet and heavily secured diplomatic zone of baridhara not far from the airport  my room was large and comfortably furnished and important as i was on business had  a desk good lighting and wifi in addition to the generous free breakfast offered the hotel has a gym and inhouse security detail  but for me the standout appeal of this hotel was the welcoming and attentive service provide by all staff  security entry reception restaurant and housekeeping   id definitely stay here again if i return to dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>stayed for a week the property is a crammed service apartment like hotel smelling of pesticides and old carpet rooms need a facelift desperately conveniently located in the diplomatic enclave of gulshan in dhaka had ordered daal fish  curry  with rice the kitchen never got it right in five nights had a misadventure with the thai food on one occasion as well staff is overworked but still cheerful that got them the second star</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>because this hotel is located in baridhara diplomatic area it is quite calm and safe compared to any other areas pickup and sending service is very helpful all staff is very kind the hotel has a great selection of breakfast of course the breakfast is delicious</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>excellent hotel to stay its located at baridhara you may avoid heavy traffic of dhaka if you have work on diplomatic zone very quite transportation is not that available hotel has its own transportation food is average</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i stayed at this hotel twice during my visits at bangladesh and although it is in a good a safe area and the staff were really friendly and accommodating i didnt really feel its matched to mark each time we stayed my colleague and i both had to change rooms for reason or another and the hotel is very noisy  and no wine so if you want an alcoholic beverage  in the evening then do your research as its hard to find in bangladesh </t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>hotels staff are very attentive to your needs and polite although communication sometimes an issue when ordering food the room is small but clean the hotel itself is a small hotel my rooms windows lookout into a wall of another building no swimming pool complimentary transport tofrom airport was very helpful traffic to the hotel is very busy at this time of the year there is hrs room service but with limited menu list breakfast was okay the hotel is good for short stay</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>i spent a couple of nights in this hotel due to the safety and its location i was picked up by the complimentary pick up service in the dhaka airport and was taken to the airport without any problems upon arrival i was checked in at the counter and there were no issues the front desk staff was courteous they had a short and brief introduction of the amenities of the hotel and told me of the hours of the breakfast buffet   the first room i received was a bit dim and and sheets were a little bit smelly like moldy smell other than that the room was clean and there was abundant hot water for the shower bottled waters and an invitation fruit plate were found on the desk  the complimentary wifi can be a bit spotty i had trouble connecting and once connected if you were</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>the hotel is located in close proximity to  diplomatic offices in a wellguarded secure and quiet neighborhood  my room was large with adequate space for the twin beds desk lounge chairs and television  the room was reasonably clean and well lit although some of the light bulbs were faulty the restaurant provides above average choice and quality of food to suit different cultures  there is also an onsite gym  the reception housekeeping and restaurant staff could not have been more attentive and helpful and on checkout the hotel waived the charges for my airport shuttle both ways which similarly was punctual and easy to use there is free and fast wifi in the rooms my only complaint was that the bed was very hard and uncomfortable and the aircon quite noisy  i</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>the hotel is tucked away in a quiet and guarded residential area which is mostly for expats it offers all the amenities which you would expect in a good hotel and an exceptional roof top restaurant which specialises in grills and barbecues  the staff is extremely helpful and considerate the gym is reasonably equipped as well  they schedule free airport pick ups and drops and have a shuttle service that runs at regular intervals</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>i stayed there several times the stuffs are professional and friendly the rooms are spacious and clean the bathroom is also up to the task never used their pool so cant say anything about that overall its a good hotel to stay</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>the service is very good at the hotel its also very neat and clean the foods are also very delicious there the place is also well maintained the room decoration is also very nice in that area please dont take a room near the lift as it may disturb you with the noise</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>stayed here for  days on business travel hotel is difficult to locate the approach is not visable at all the amenities and the room condition is not up to the mark the plug points were not functional and room was not hygenic</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>the restaurant is good with delicious food location is also good it is situated in diplomatic zone  called baridhara of dhaka it is situated in a very convenient place though public transport is hard to hail</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>this hotel is situated in high security area of baridhara diplomatic compound this area houses many high commissions and house of high commissioners as a result area is but secluded hotel is very good a very modern business hotel with all standard amenities</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>the rooms and service are good the staff are polite and courteous  i wouldnt rate the location highly as it is in the middle of a residential area and there are no commercial establishments other restaurants within walking distance and any other transport except bikes could mean  minutes in dhaka traffic they did not offer a complimentary  airport pickup though a previous traveller claims to have received it did not like the breakfast here at all  the gym is a small crowded room with old equipment  the treadmill seemed it could break any moment</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>conducted a training workshop on th floor of the hotel the training room is very basic but the greenery on the terrace outside the training room is very pleasant and makes for very good break away space worth mentioning is the excellent service provided by the restaurant manager alam and his team alam is extremely enthusiastic  energetic proactive  and positive energy person  i am a vegetarian and enjoyed the non spicy vegetarian dishes they served on special request</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>i checked into the hotel for a one night stay they offered complimentary airport pick up and drop very impressed by the boutique hotel i have been a frequent visitor to dhaka and trying to get a good hotel my search ended once i stayed here they have another hotel ascott palace the manager took me to that as well and i am impressed by the quality of their interiors i am sure to be back in the hotel next time i am in dhaka</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>location is nice as it is close to airport and being in diplomatic area place is quiet and clean however every location of my clients place though was within range of  kms but it took lot of time to reach due to heavy traffic which doesnt move private taxi taken from hotel is very costly internet connectivity was good and so was staff very hospitable overall experience was good</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>nearby the airport  minutes depending of the traffic jam the ascott hotel has all the faculty that you need for a short stay except the pool small restaurant and a small spa but very comfortable rooms are new clean and enough large</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>pro   very friendly staff and area  contra  totally overpriced rooms smelly room very smelly corridor room for sure not m old interior old design old shower curtain very small windows no nice view out of window all dark design rip off  gym not state of the art as promised in the internet broken edges jacuzzi not working see the photo lol   i not recommend and will not stay again apologies for the very friendly staff but what you get is one of the worst rip offs in history i do not expect  stars rooms the price of usd night are a joke at least the everything should be well maintained and it was not</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>a quaint but very hospitable hotel where the staff treat you like family if it werent for the weak internet link for one day i would have given it an excellent the staff were very helpful and even gave me additional coffee and fruits</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>this is a very good hotel with an excellent location in road  baridhara close to gulshan  and close to many embassies and the gulshanbanani business districts the service is excellent rooms very good and nice meals available from breakfast to dinner there is a smallish conference centre and a pleasant roof top dinner area next to the spa and fitness centre which are both very good my only concern with the ascott is the price getting just a little expensive compared to some of the more affordable options available in the same district but it does still represent very good value for money and id have no hesitation in recommending it to anyone on a medium size budget the spa is also getting expensive so i now look for other alternatives close by</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>i was on a business trip to dhaka and decided after reading some reviews to book into the ascott the rooms are spacious and clean with ample closet space for all my shirts and trousers the staff are very friendly and can not do enough to help make my stay enjoyable  the is a free collection and drop off available which saves on haggling over taxi cost the food is well prepared and having paid for breakfast not limited to the selection provided not keen on curry and noodles first thing  all in all a very enjoyable stay and quite prepared to go back on my next trip  with a short taxi ride or paying for the in house transport there is attractions local would not suggest walking at night as poorly lit and the roadspaths are a in a state of disrepair</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">this is my first time travel to dhaka with my  colleagues for business and stay for  days the staffs are very friendly and polite the hotel is clean and the food is quite good the customer care joan is very friendly and helpful always lend help and advise us about places to visit etc this place is quiet just the construction next the hotel is on going somehow disturber anyways still acceptable as you will not staying in the hotel all the time hopefully we will be staying at the same hotel for the next visit hope to see you again joan peggy mee and lily will miss you </t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>i frequently come to dhaka for business and stay for a month at a time i find the ascott residence staff always eager to please and the hotel is kept very clean the rooms have everything that you might need for a long or short stay i have found the food to be quite excellent but after trying everything and staying for long periods the odd change is always welcome joanna who works in marketing has many great suggestions for outside restaurant experiences she takes extra care to insure that every customer is as happy as they can be when away from home the hotel is located in the diplomat district so safety never feels like a concern over all im quite happy and plan to say at the ascott for my next visit</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>this is the second time as a school we stay at ascott residence and it was awesome we realy enjoyed are stay at ascott your staff was very professional and very supportive only the tv channels needs to be more internationals then local or indian hope to see you guys again  thanks qadeer</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">staff is very cooperative rooms are neatly maintainedif you are an indian then even they arrange veg stuff you requirefrom the restaurant purnima sonia faruque well mannered they take care of you on personal level secured place and located in calm and quite areagulshan commercial area is very close by you get all sort of helpfrom the staffno problems in short the only point price wise its bit costlier </t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i was here for  days business trip and our client booked our accommodation at ascott which has a very good location a walking distance to my workplace and it is located in diplomatic zone area so its safe the staff are very polite courteous and friendly joanna who is their customer relations officer is also very friendly and she make sure that all guests are comfortable she is a very nice lady a little suggestion the breakfast menu is always the same imagine for  days i stayed at the hotel its the same food everyday put a bit of variation and maybe every week change the menu </t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>this is no way a  star hotel i dont know how this hotel has been given  star i changed  rooms first room it was stinking second room the aircon was making too much noise hence they shifted my room at  am in the morning very bad experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>stayed here for one night on business the ascott is an international serviced residence brand from singapore and they are branded midhigh range therefore i certainly was not expecting the very basic setup of the room clean and wellkept but very basic   the room layout is what you would expect of a serviced apartment with a small dry kitchen living room bedroom and bathroom i was on the nd floor so the sound of traffic and people walking about went on quite late into the night   the bed was also hard and the bedsheets were basic safe to say i did not have the best sleep   i did not have time to eat breakfast at the hotel   everybody in bangladesh is very friendly and helpful so it was nice to know that the hotel kept to this standard</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>overall i can say that my stay was quite good a bit better than when i stayed in the same hotel  years ago  it has all the basic amenities and services and it is very near my workplace  if theres one thing that i liked the best its the shower because the water is strong and the temp is easy to control  the staff are also generally courteous warm and helpful  the breakfast and menu can be improved though  the selection is quite limited and if you have stayed for almost  weeks you will surely get tired of the food  there are times that some staff at the restaurant have the tendency to be a bit selective when serving people of different nationalities and tend to favor one over the other   there are no other restaurants near the hotel so if youre craving for other</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>i stayed here with my whole family for three nights when we could not get into our usual hotel in gulshan  the hotel looks fine from the outside but inside has a upmarket feeling lobby  i was staying with my husband and  year old daughter and had a  bedroom suite  the bedroom had two double beds and was very big and beautifully decorated  we also had a a sizable living room and kitchen area making it easy to make tea for the whole group  the other twin rooms were all decorated to the same high standard but were slightly smaller  the bedding ll looked and felt luxurious made the rooms look good and the beds were very comfortable  the walls were pretty think and so we had to try and talk quietly to avoid being heard outside  the rooms were very quiet with no noise</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>i stayed at the ascott last month while returning back from an official trip i was pleasantly surprised as soon as i entered the hotel because from the outside it looks quite a small place but it very well equipped like any other big hotel the rooms were extremely spacious  comfortable enough there is complimentary wifiwhich was a bit problematic during my stay tv with dth facilities fruit baskets  other basic necessities shower was well equipped  good enough in case you smoke youd have to ask for the smoking rooms the staff is very helpful  very polite  extra browny points for the amazing morning breakfast spread food at both the restraunts was amazing highly recommended over other high priced options in the baridhara area</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>the hotel is quiet and clean and cost represnets value for money  i had basic bedroom which was a reaonalbe size with an armchair to watch tv  the bed was ok but rather hard  shower excellent  if you dont like smoke go for roons starting with a  in the number which is a bit confusing as they are on the th floor  food is ok and again not expensive for a hotel  coffee could be better and no alcohol served but you can bring take in</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">its a small hotel but it do have almost everything similar to any bigger hotel but do take note there is some renovations taking place behind the hotel so it could be noisy my room was upgraded to the royal suite which is extremely spacious with a kitchen area though i have not much use as its a business trip the hotel restaurant give me a local canned drink but charged me a imported can drink price which is like  bucks sgd which i think should not happen </t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>we stayed there in september attending a friends wedding in dhaka the hotel is located in an upmarket district of dhaka very quiet green and close to the airport it is very well decorated and all staff speak good english excellent rooms good facilities and overall we had a very pleasant time there recommended</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>i stayed in a deluxe roomrooms are very clean and  also shower had a excelent water fallthe hotel is in diplomatic zone which means extra safetythe food was ok  but improve the room serve still bettervery noisy sorroundings due to some breakage of near by buildings</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">having stayed on a number of occasions and found everything ok staff very welcomingrooms are clean and well maintained a problem with the restaurant in that my order took over  mins to arrive having ordered a basic shaslik and chips </t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>my nd stay here the ascott is very near thengo i work for rooms are no frills clean bed is okay food is average competent and friendly front desk staff the hotel is in the diplomatic zone which means there are no commercial facilities close by traffic in dhaka is bad and it can take  minutes to get somewhere a mile away by car theres a rooftop restaurant and a small gym on te premises</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>room   very clean with all the amenities you need  i stayed in a deluxe room which is not the best but not the worst   shower had excellent water flow and hotcold was easily adjusted to suit preference   many outlets to charge devices and free wifi recommend bringing multiple adaptors   bed had very hard mattress but sheets were good quality soft and comfortable   windows were not sealed tightly and therefore not sound proof which allowed construction noise to come through room beware construction couninues all night   lcd flat screen tv with over  channels many of which were english speaking or subtitled   very good adjustable air conditioning actually had to turn it down  service   excellent   staff were very friendly and accomodating   hotel kept very</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>small hotel with great service i felt like beeing home the personnel is very helpful and friendly food can be customized since im not fan of spicy food that is served in this part of the world but they made it no spicy for me without any problems hotel is placed in good neighborhood without crime and big noise of the traffic   overall very good and more than expected</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>stayed over on route home the hotel is in a safe area of the embassies on arrival the staff were very friendly and efficient my booking was dealt with quickly on arrival in my room found it very clean with coffee facilities and a good shower after  hours on the road traveling this was a good start</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>the facilities include free pickup from and drop to  the airport which is not too far from the hotel the interior of the hotel is nice and it is located at a residential area where no shops are available nearby no shop not even a  barber shop is inside the hotel the staff members are wellbehaved and cooperative but despite all compared to the price which is nearly us   for  a room per night including vat and service charges the accommodation is not in my judgment worth the money at all</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>in the quiet and safe heart of baridhara i had a suite for a lengthy stay and found the room spacious although the bed was quite hard the staff were pleasent and helpful the breakfast was more than adequate adequate</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>the reason i rate it poor because personally feel the hotel does not have  star feel  personally counter several unhappy situation however fixed by hotels management i felt i had paid to learn the lesson   pro  ascott the residence won two awards from other country which i dont know what award is that but it sound great  room equip with lcd tv with more than  tv channel  provided ml water each day from room cleaner   free news paper for each day  fix complain before next cob day   free shuttle tofrom dhaka airport   alot of power socket point         mini fridge is available         independent air cond unitwhich you can adjust your own preference temperature  cons  terrible internet speed difficulty with skype call during peak hour  dont</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>certainly not a hotel to stay at if you are an antismoker the rooms smell strongly of stale cigarette smoke not pleasant bedroom comfortable but bathroom facilities not good i was very disappointed by breakfast i have been travelling a lot in recent months for work and this is the first hotel i can think of where breakfast was lacking  poor choice of food and what was on display was not great i didnt eat in the restaurant for dinner but had room service on my last night food very mediocre fries inedible  the plus side lovely staff reception clean and pleasant and most importantly i felt very safe but definitely not my choice of hotel</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>the stay is ok bfast is ok airport shuttle is provided foc the only downside on the last day when about to check out they charge me for room for which i already paid via website ive been premier member of that website and i explain everything already paid the staff told me i maybe paid the website but the website havent pay to the hotel  it took  staff including the manager to check and  minutes waiting finally they told me everything is ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">if you have no other options and if you have business in the bardhara district then this is a good place to stay  i stayed here for three weeks  for the first week i stay in a royal suite on the th floor  for the last two weeks i stayed in a premium room  both were fine  clean and wellsprayed to ward off mosquitoes  i would have preferred the suite for such a long stay if it werent so dark  it faced other buildings so the view was terrible but it was quieter  the premium room was actually quite nice  it faced the street and even though i heard street noise the daylight and sunrise were lovely  the dilemma was the mosque was only half a block away  prayer calls at am were surprising at first but then you get used to it like all other things about dhaka </t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>found the hotel lacking in many aspects   the rooms were of ok size but had mosquites  the bathrooms were a little low on lighting   hot water took ages once the shower was turned on  the mosquito spray led to dead roaches turning up in the room  the breakfast was pretty limited in its offering  the best part of the hotel was the rooftop bbq which served good quality food though a tad expensive</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>if you are willing to have a long stay at dhaka ascott is the right place the staffs are quite warm  rooms are comfortable fooding is always a challange as they have very limited menu since it si located in diplomatic zone of dhaka so outside of environment looks very safe</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>a very poor quality hotel with claustrophobic rooms and bad toilets service was missing and in spite of a high charge even a mini bar or kitchenette was missing food was very costly the  staff at the reception was non communicative and confused i was charged for a breakfast which was supposed to be complimentary</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">true residence with almost family atmosphere hotel is new and clean service is friendly and social  diner at night is fine choice of asian a la carte and buffet a la carte takes  minutes to bring first dish breakfast is warm asian buffet lacks some western options  despite quite area thin walls and windows allow for some disturbance at night  for dhaka area this is a very attractive alternative to raddisson and westin unless you expect not less than </t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>ascott the residence opened in april  there were a good choice of rooms all well furnished and very clean rooms are light airy and spacious i stayed in a superior double the only downside being the ac blew onto the bed the free internet is wireless the food in the restaurant was good although not all items on the menu are available the staff were pleasant but not really on the ball  overall it is a good hotel i would definately recommend and stay there again with pleasure</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>